<commit_message>
Added Final Batch of Data From Azure, Part 2
</commit_message>
<xml_diff>
--- a/docs/data.xlsx
+++ b/docs/data.xlsx
@@ -8,14 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\USERDATA\chevrotain\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BE7F7B1-14E2-4F55-89FE-E58723643D6B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7929865F-A29A-443A-AB33-F143B0ABFD68}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{A210CDE5-00A4-40CA-8B46-4EB7639998ED}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{A210CDE5-00A4-40CA-8B46-4EB7639998ED}"/>
   </bookViews>
   <sheets>
     <sheet name="Zero" sheetId="1" r:id="rId1"/>
     <sheet name="CmRDTO" sheetId="2" r:id="rId2"/>
     <sheet name="CvRDT" sheetId="3" r:id="rId3"/>
+    <sheet name="5Repl" sheetId="4" r:id="rId4"/>
+    <sheet name="7Repl" sheetId="6" r:id="rId5"/>
+    <sheet name="1Repl" sheetId="5" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="8">
   <si>
     <t>10ops/s</t>
   </si>
@@ -559,7 +562,7 @@
         <v>25</v>
       </c>
       <c r="Q2" s="6">
-        <f t="shared" ref="Q2:Q6" si="0">1000/P2</f>
+        <f t="shared" ref="Q2:Q4" si="0">1000/P2</f>
         <v>40</v>
       </c>
     </row>
@@ -1273,7 +1276,7 @@
   <dimension ref="A1:O23"/>
   <sheetViews>
     <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="M17" sqref="M17"/>
+      <selection activeCell="M17" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1959,7 +1962,7 @@
         <v>1131.5806022222223</v>
       </c>
       <c r="J23" s="1">
-        <f t="shared" ref="J23:K23" si="7">AVERAGE(J14:J22)</f>
+        <f t="shared" ref="J23" si="7">AVERAGE(J14:J22)</f>
         <v>30.873285555555558</v>
       </c>
       <c r="K23" s="1"/>
@@ -1973,8 +1976,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2884177-FD20-46D4-A2A8-57BEA1054E7C}">
   <dimension ref="A1:O23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="N13" sqref="N13"/>
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="N13" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2611,4 +2614,1156 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B8F6C9B-5F1D-4F14-BF34-282173FE9481}">
+  <dimension ref="A1:O24"/>
+  <sheetViews>
+    <sheetView topLeftCell="A4" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I1" t="s">
+        <v>2</v>
+      </c>
+      <c r="M1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>119.36660999999999</v>
+      </c>
+      <c r="B2">
+        <v>100</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>84.965299999999999</v>
+      </c>
+      <c r="F2">
+        <v>100</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="I2">
+        <v>98.861915999999994</v>
+      </c>
+      <c r="J2">
+        <v>95.370930000000001</v>
+      </c>
+      <c r="M2">
+        <v>126.80374</v>
+      </c>
+      <c r="N2">
+        <v>90.589714000000001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>168.52742000000001</v>
+      </c>
+      <c r="B3">
+        <v>100</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>163.54854</v>
+      </c>
+      <c r="F3">
+        <v>100</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <v>160.93306000000001</v>
+      </c>
+      <c r="J3">
+        <v>85.396649999999994</v>
+      </c>
+      <c r="M3">
+        <v>201.55536000000001</v>
+      </c>
+      <c r="N3">
+        <v>10.14218</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>86.222329999999999</v>
+      </c>
+      <c r="B4">
+        <v>100</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>123.01479</v>
+      </c>
+      <c r="F4">
+        <v>100</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <v>202.06862000000001</v>
+      </c>
+      <c r="J4">
+        <v>100</v>
+      </c>
+      <c r="M4">
+        <v>240.99596</v>
+      </c>
+      <c r="N4">
+        <v>32.653060000000004</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>205.37432999999999</v>
+      </c>
+      <c r="B5">
+        <v>100</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>204.97629000000001</v>
+      </c>
+      <c r="F5">
+        <v>100</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <v>139.92080000000001</v>
+      </c>
+      <c r="J5">
+        <v>100</v>
+      </c>
+      <c r="M5">
+        <v>204.01442</v>
+      </c>
+      <c r="N5">
+        <v>5.5378059999999998</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>179.60724999999999</v>
+      </c>
+      <c r="B6">
+        <v>100</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>179.74464</v>
+      </c>
+      <c r="F6">
+        <v>100</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <v>190.22971999999999</v>
+      </c>
+      <c r="J6">
+        <v>100</v>
+      </c>
+      <c r="M6">
+        <v>134.82889</v>
+      </c>
+      <c r="N6">
+        <v>7.779172</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>117.483734</v>
+      </c>
+      <c r="B7">
+        <v>100</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>84.030829999999995</v>
+      </c>
+      <c r="F7">
+        <v>100</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="I7">
+        <v>86.8386</v>
+      </c>
+      <c r="J7">
+        <v>100</v>
+      </c>
+      <c r="M7">
+        <v>122.79678</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>161.47450000000001</v>
+      </c>
+      <c r="B8">
+        <v>100</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>162.97765000000001</v>
+      </c>
+      <c r="F8">
+        <v>100</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <v>166.0779</v>
+      </c>
+      <c r="J8">
+        <v>100</v>
+      </c>
+      <c r="M8">
+        <v>193.90903</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>80.461005999999998</v>
+      </c>
+      <c r="B9">
+        <v>100</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>118.38558999999999</v>
+      </c>
+      <c r="F9">
+        <v>100</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="I9">
+        <v>122.48195</v>
+      </c>
+      <c r="J9">
+        <v>100</v>
+      </c>
+      <c r="M9">
+        <v>132.84200000000001</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>204.72522000000001</v>
+      </c>
+      <c r="B10">
+        <v>100</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>204.38390000000001</v>
+      </c>
+      <c r="F10">
+        <v>100</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="I10">
+        <v>234.03287</v>
+      </c>
+      <c r="J10">
+        <v>81.441670000000002</v>
+      </c>
+      <c r="M10">
+        <v>212.17934</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>181.15341000000001</v>
+      </c>
+      <c r="B11">
+        <v>100</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>179.80916999999999</v>
+      </c>
+      <c r="F11">
+        <v>100</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="I11">
+        <v>180.55073999999999</v>
+      </c>
+      <c r="J11">
+        <v>81.441670000000002</v>
+      </c>
+      <c r="M11">
+        <v>227.16487000000001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <f>AVERAGE(A2:A11)</f>
+        <v>150.439581</v>
+      </c>
+      <c r="B12" s="1">
+        <f>AVERAGE(B2:B10)</f>
+        <v>100</v>
+      </c>
+      <c r="C12" s="1">
+        <f>AVERAGE(C2:C10)</f>
+        <v>0</v>
+      </c>
+      <c r="E12" s="1">
+        <f>AVERAGE(E2:E11)</f>
+        <v>150.58367000000004</v>
+      </c>
+      <c r="F12" s="1">
+        <f>AVERAGE(F2:F10)</f>
+        <v>100</v>
+      </c>
+      <c r="G12" s="1">
+        <f>AVERAGE(G2:G10)</f>
+        <v>0</v>
+      </c>
+      <c r="I12" s="1">
+        <f>AVERAGE(I2:I11)</f>
+        <v>158.19961760000001</v>
+      </c>
+      <c r="J12" s="1">
+        <f>AVERAGE(J2:J10)</f>
+        <v>95.801027777777776</v>
+      </c>
+      <c r="K12" s="1" t="e">
+        <f>AVERAGE(K2:K10)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M12" s="1">
+        <f>AVERAGE(M2:M11)</f>
+        <v>179.70903900000002</v>
+      </c>
+      <c r="N12" s="1">
+        <f>AVERAGE(N2:N10)</f>
+        <v>29.340386399999993</v>
+      </c>
+      <c r="O12" s="1" t="e">
+        <f>AVERAGE(O2:O10)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>3</v>
+      </c>
+      <c r="E13" t="s">
+        <v>4</v>
+      </c>
+      <c r="I13" t="s">
+        <v>5</v>
+      </c>
+      <c r="M13" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>254.64157</v>
+      </c>
+      <c r="E14">
+        <v>382.90143</v>
+      </c>
+      <c r="I14">
+        <v>815.56039999999996</v>
+      </c>
+      <c r="M14">
+        <v>237.34558000000001</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>179.26820000000001</v>
+      </c>
+      <c r="E15">
+        <v>333.50002999999998</v>
+      </c>
+      <c r="I15">
+        <v>903.71</v>
+      </c>
+      <c r="M15">
+        <v>349.06569999999999</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>436.71782999999999</v>
+      </c>
+      <c r="E16">
+        <v>220.44884999999999</v>
+      </c>
+      <c r="I16">
+        <v>1305.4963</v>
+      </c>
+      <c r="M16">
+        <v>384.66385000000002</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>219.52202</v>
+      </c>
+      <c r="E17">
+        <v>245.99455</v>
+      </c>
+      <c r="I17">
+        <v>1876.0728999999999</v>
+      </c>
+      <c r="M17">
+        <v>236.74377000000001</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>200.35748000000001</v>
+      </c>
+      <c r="E18">
+        <v>1110.2077999999999</v>
+      </c>
+      <c r="I18">
+        <v>3337.7964000000002</v>
+      </c>
+      <c r="M18">
+        <v>343.524</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>91.794479999999993</v>
+      </c>
+      <c r="E19">
+        <v>299.80444</v>
+      </c>
+      <c r="I19">
+        <v>978.00340000000006</v>
+      </c>
+      <c r="M19">
+        <v>387.58249999999998</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>91.794479999999993</v>
+      </c>
+      <c r="E20">
+        <v>316.95929999999998</v>
+      </c>
+      <c r="I20">
+        <v>1325.6438000000001</v>
+      </c>
+      <c r="M20">
+        <v>245.69693000000001</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>194.32339999999999</v>
+      </c>
+      <c r="B21" s="2"/>
+      <c r="E21">
+        <v>926.90560000000005</v>
+      </c>
+      <c r="I21">
+        <v>1268.2029</v>
+      </c>
+      <c r="M21">
+        <v>341.67189999999999</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>197.14722</v>
+      </c>
+      <c r="E22">
+        <v>817.74170000000004</v>
+      </c>
+      <c r="I22">
+        <v>2949.2366000000002</v>
+      </c>
+      <c r="M22">
+        <v>386.97719999999998</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>217.35345000000001</v>
+      </c>
+      <c r="E23">
+        <v>1232.9989</v>
+      </c>
+      <c r="I23">
+        <v>6293.4472999999998</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A24" s="1">
+        <f>AVERAGE(A14:A23)</f>
+        <v>208.29201300000005</v>
+      </c>
+      <c r="B24" s="1" t="e">
+        <f>AVERAGE(B14:B22)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C24" s="1" t="e">
+        <f>AVERAGE(C14:C22)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E24" s="1">
+        <f>AVERAGE(E14:E23)</f>
+        <v>588.74626000000012</v>
+      </c>
+      <c r="F24" s="1" t="e">
+        <f>AVERAGE(F14:F22)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G24" s="1" t="e">
+        <f>AVERAGE(G14:G22)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I24" s="1">
+        <f>AVERAGE(I14:I22)</f>
+        <v>1639.969188888889</v>
+      </c>
+      <c r="J24" s="1" t="e">
+        <f>AVERAGE(J14:J22)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K24" s="1" t="e">
+        <f>AVERAGE(K14:K22)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91B31920-5678-46E4-B10A-2BE11E7DA4AF}">
+  <dimension ref="A1:O23"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="P3" sqref="P3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I1" t="s">
+        <v>2</v>
+      </c>
+      <c r="M1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>92.648049999999998</v>
+      </c>
+      <c r="B2">
+        <v>100</v>
+      </c>
+      <c r="E2">
+        <v>163.09805</v>
+      </c>
+      <c r="F2">
+        <v>100</v>
+      </c>
+      <c r="I2">
+        <v>105.21686</v>
+      </c>
+      <c r="J2">
+        <v>100.92867</v>
+      </c>
+      <c r="M2">
+        <v>140.32820000000001</v>
+      </c>
+      <c r="N2">
+        <v>180.88050999999999</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>163.22436999999999</v>
+      </c>
+      <c r="E3">
+        <v>120.15487</v>
+      </c>
+      <c r="I3">
+        <v>924.68604000000005</v>
+      </c>
+      <c r="J3">
+        <v>177.19792000000001</v>
+      </c>
+      <c r="M3">
+        <v>155.36487</v>
+      </c>
+      <c r="N3">
+        <v>211.52930000000001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>126.10741400000001</v>
+      </c>
+      <c r="E4">
+        <v>88.296689999999998</v>
+      </c>
+      <c r="I4">
+        <v>177.23541</v>
+      </c>
+      <c r="J4">
+        <v>191.17116999999999</v>
+      </c>
+      <c r="M4">
+        <v>216.03958</v>
+      </c>
+      <c r="N4">
+        <v>169.51566</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>208.24869000000001</v>
+      </c>
+      <c r="E5">
+        <v>207.3245</v>
+      </c>
+      <c r="I5">
+        <v>1006.2138</v>
+      </c>
+      <c r="J5">
+        <v>128.51257000000001</v>
+      </c>
+      <c r="M5">
+        <v>231.02274</v>
+      </c>
+      <c r="N5">
+        <v>144.0771</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>119.5558</v>
+      </c>
+      <c r="E6">
+        <v>125.821556</v>
+      </c>
+      <c r="I6">
+        <v>222.67355000000001</v>
+      </c>
+      <c r="J6">
+        <v>216.57210000000001</v>
+      </c>
+      <c r="M6">
+        <v>141.61689999999999</v>
+      </c>
+      <c r="N6">
+        <v>509.88112999999998</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>180.99083999999999</v>
+      </c>
+      <c r="E7">
+        <v>171.47632999999999</v>
+      </c>
+      <c r="I7">
+        <v>167.50496999999999</v>
+      </c>
+      <c r="J7">
+        <v>123.22119000000001</v>
+      </c>
+      <c r="M7">
+        <v>231.8398</v>
+      </c>
+      <c r="N7">
+        <v>214.86998</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>166.15163999999999</v>
+      </c>
+      <c r="E8">
+        <v>179.10829000000001</v>
+      </c>
+      <c r="I8">
+        <v>125.885796</v>
+      </c>
+      <c r="J8">
+        <v>188.64797999999999</v>
+      </c>
+      <c r="M8">
+        <v>228.24737999999999</v>
+      </c>
+      <c r="N8">
+        <v>195.74275</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <f>AVERAGE(A2:A10)</f>
+        <v>150.98954342857141</v>
+      </c>
+      <c r="B11" s="1">
+        <f t="shared" ref="B11:C11" si="0">AVERAGE(B2:B10)</f>
+        <v>100</v>
+      </c>
+      <c r="C11" s="1" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E11" s="1">
+        <f>AVERAGE(E2:E10)</f>
+        <v>150.75432657142855</v>
+      </c>
+      <c r="F11" s="1">
+        <f t="shared" ref="F11:G11" si="1">AVERAGE(F2:F10)</f>
+        <v>100</v>
+      </c>
+      <c r="G11" s="1" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I11" s="1">
+        <f>AVERAGE(I2:J10)</f>
+        <v>275.40485900000004</v>
+      </c>
+      <c r="J11" s="1">
+        <f t="shared" ref="J11:K11" si="2">AVERAGE(J2:J10)</f>
+        <v>160.89308571428572</v>
+      </c>
+      <c r="K11" s="1" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M11" s="1">
+        <f>AVERAGE(M2:N10)</f>
+        <v>212.21113571428569</v>
+      </c>
+      <c r="N11" s="1"/>
+      <c r="O11" s="1" t="e">
+        <f t="shared" ref="N11:O11" si="3">AVERAGE(O2:O10)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>3</v>
+      </c>
+      <c r="E13" t="s">
+        <v>4</v>
+      </c>
+      <c r="I13" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>178.46017000000001</v>
+      </c>
+      <c r="B14">
+        <v>113.87115</v>
+      </c>
+      <c r="E14">
+        <v>215.39850999999999</v>
+      </c>
+      <c r="F14">
+        <v>769.81903</v>
+      </c>
+      <c r="I14">
+        <v>953.49559999999997</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>204.95529999999999</v>
+      </c>
+      <c r="B15">
+        <v>154.07105999999999</v>
+      </c>
+      <c r="E15">
+        <v>591.22253000000001</v>
+      </c>
+      <c r="F15">
+        <v>251.30181999999999</v>
+      </c>
+      <c r="I15">
+        <v>2317.8874999999998</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>143.39938000000001</v>
+      </c>
+      <c r="B16">
+        <v>447.10977000000003</v>
+      </c>
+      <c r="E16">
+        <v>498.62975999999998</v>
+      </c>
+      <c r="F16">
+        <v>208.06496999999999</v>
+      </c>
+      <c r="I16">
+        <v>1624.6404</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>212.25667999999999</v>
+      </c>
+      <c r="B17">
+        <v>233.71455</v>
+      </c>
+      <c r="E17">
+        <v>335.49441999999999</v>
+      </c>
+      <c r="F17">
+        <v>274.86093</v>
+      </c>
+      <c r="I17">
+        <v>2448.3717999999999</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>192.72461000000001</v>
+      </c>
+      <c r="B18">
+        <v>185.05974000000001</v>
+      </c>
+      <c r="E18">
+        <v>227.24321</v>
+      </c>
+      <c r="F18">
+        <v>675.97850000000005</v>
+      </c>
+      <c r="I18">
+        <v>2088.31</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>239.8597</v>
+      </c>
+      <c r="B19">
+        <v>216.07745</v>
+      </c>
+      <c r="E19">
+        <v>1477.5824</v>
+      </c>
+      <c r="F19">
+        <v>1120.2248999999999</v>
+      </c>
+      <c r="I19">
+        <v>1912.3741</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="E20">
+        <v>1755.8889999999999</v>
+      </c>
+      <c r="F20">
+        <v>1278.3921</v>
+      </c>
+      <c r="I20">
+        <v>5043.7079999999996</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A23" s="1">
+        <f>AVERAGE(A14:B22)</f>
+        <v>210.12996333333331</v>
+      </c>
+      <c r="B23" s="1"/>
+      <c r="C23" s="1" t="e">
+        <f t="shared" ref="B23:C23" si="4">AVERAGE(C14:C22)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E23" s="1">
+        <f>AVERAGE(E14:F22)</f>
+        <v>691.43586285714287</v>
+      </c>
+      <c r="F23" s="1">
+        <f t="shared" ref="F23:G23" si="5">AVERAGE(F14:F22)</f>
+        <v>654.09174999999993</v>
+      </c>
+      <c r="G23" s="1" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I23" s="1">
+        <f>AVERAGE(I14:I22)</f>
+        <v>2341.2553428571423</v>
+      </c>
+      <c r="J23" s="1" t="e">
+        <f t="shared" ref="J23" si="6">AVERAGE(J14:J22)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K23" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D20F941F-E03D-4830-A52F-A84B60AFDE39}">
+  <dimension ref="A1:O23"/>
+  <sheetViews>
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="E21" sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I1" t="s">
+        <v>2</v>
+      </c>
+      <c r="M1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>83.850684999999999</v>
+      </c>
+      <c r="E2">
+        <v>120.46129999999999</v>
+      </c>
+      <c r="I2">
+        <v>223.51424</v>
+      </c>
+      <c r="M2">
+        <v>432.11223999999999</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>86.655640000000005</v>
+      </c>
+      <c r="E3">
+        <v>120.82997</v>
+      </c>
+      <c r="I3">
+        <v>340.50146000000001</v>
+      </c>
+      <c r="M3">
+        <v>487.02769999999998</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>82.150689999999997</v>
+      </c>
+      <c r="E4">
+        <v>121.99661999999999</v>
+      </c>
+      <c r="I4">
+        <v>237.03716</v>
+      </c>
+      <c r="M4">
+        <v>85.050330000000002</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <f>AVERAGE(A2:A10)</f>
+        <v>84.219004999999996</v>
+      </c>
+      <c r="B11" s="1" t="e">
+        <f t="shared" ref="B11:C11" si="0">AVERAGE(B2:B10)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C11" s="1" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E11" s="1">
+        <f>AVERAGE(E2:E10)</f>
+        <v>121.09596333333333</v>
+      </c>
+      <c r="F11" s="1" t="e">
+        <f t="shared" ref="F11:G11" si="1">AVERAGE(F2:F10)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G11" s="1" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I11" s="1">
+        <f>AVERAGE(I2:I10)</f>
+        <v>267.01762000000002</v>
+      </c>
+      <c r="J11" s="1" t="e">
+        <f t="shared" ref="J11:K11" si="2">AVERAGE(J2:J10)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K11" s="1" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M11" s="1">
+        <f>AVERAGE(M2:M10)</f>
+        <v>334.73009000000002</v>
+      </c>
+      <c r="N11" s="1" t="e">
+        <f t="shared" ref="N11:O11" si="3">AVERAGE(N2:N10)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O11" s="1" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>3</v>
+      </c>
+      <c r="E13" t="s">
+        <v>4</v>
+      </c>
+      <c r="I13" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>679.57420000000002</v>
+      </c>
+      <c r="E14">
+        <v>90.202659999999995</v>
+      </c>
+      <c r="I14">
+        <v>2007.2598</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>644.83185000000003</v>
+      </c>
+      <c r="E15">
+        <v>1540.0369000000001</v>
+      </c>
+      <c r="I15">
+        <v>651.56035999999995</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>83.307784999999996</v>
+      </c>
+      <c r="E16">
+        <v>290.16521999999998</v>
+      </c>
+      <c r="I16">
+        <v>600.42610000000002</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A23" s="1">
+        <f>AVERAGE(A14:A22)</f>
+        <v>469.23794500000002</v>
+      </c>
+      <c r="B23" s="1" t="e">
+        <f t="shared" ref="B23:C23" si="4">AVERAGE(B14:B22)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C23" s="1" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E23" s="1">
+        <f>AVERAGE(E14:E22)</f>
+        <v>640.13492666666662</v>
+      </c>
+      <c r="F23" s="1" t="e">
+        <f t="shared" ref="F23:G23" si="5">AVERAGE(F14:F22)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G23" s="1" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I23" s="1">
+        <f>AVERAGE(I14:I22)</f>
+        <v>1086.41542</v>
+      </c>
+      <c r="J23" s="1" t="e">
+        <f t="shared" ref="J23" si="6">AVERAGE(J14:J22)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K23" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Final Version of The Report
</commit_message>
<xml_diff>
--- a/docs/data.xlsx
+++ b/docs/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\USERDATA\chevrotain\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7929865F-A29A-443A-AB33-F143B0ABFD68}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B33B140-8942-4F60-BCEA-D3107C0616FB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{A210CDE5-00A4-40CA-8B46-4EB7639998ED}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{A210CDE5-00A4-40CA-8B46-4EB7639998ED}"/>
   </bookViews>
   <sheets>
     <sheet name="Zero" sheetId="1" r:id="rId1"/>
@@ -1276,7 +1276,7 @@
   <dimension ref="A1:O23"/>
   <sheetViews>
     <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="M17" sqref="A1:XFD1048576"/>
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1976,8 +1976,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2884177-FD20-46D4-A2A8-57BEA1054E7C}">
   <dimension ref="A1:O23"/>
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="N13" sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2351,8 +2351,8 @@
         <v>99.858228888888888</v>
       </c>
       <c r="G11" s="1">
-        <f t="shared" si="1"/>
-        <v>1.6666666666666667</v>
+        <f>AVERAGE(G2:G10)/1.4</f>
+        <v>1.1904761904761907</v>
       </c>
       <c r="I11" s="1">
         <f>AVERAGE(I2:I10)</f>
@@ -2363,8 +2363,8 @@
         <v>92.956221555555558</v>
       </c>
       <c r="K11" s="1">
-        <f>AVERAGE(K2:K10)</f>
-        <v>15</v>
+        <f>AVERAGE(K2:K10)/1.4</f>
+        <v>10.714285714285715</v>
       </c>
       <c r="M11" s="1">
         <f>AVERAGE(M2:M10)</f>
@@ -2375,8 +2375,8 @@
         <v>92.317340000000002</v>
       </c>
       <c r="O11" s="1">
-        <f>AVERAGE(O2:O10)</f>
-        <v>92.5</v>
+        <f>AVERAGE(O2:O10)/1.4</f>
+        <v>66.071428571428569</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
@@ -2583,8 +2583,8 @@
         <v>85.67499022222222</v>
       </c>
       <c r="C23" s="1">
-        <f t="shared" si="2"/>
-        <v>51.666666666666664</v>
+        <f>AVERAGE(C14:C22)/1.4</f>
+        <v>36.904761904761905</v>
       </c>
       <c r="E23" s="1">
         <f>AVERAGE(E14:E22)</f>
@@ -2609,6 +2609,10 @@
       <c r="K23" s="1" t="e">
         <f t="shared" si="4"/>
         <v>#DIV/0!</v>
+      </c>
+      <c r="M23">
+        <f>AVERAGE(M14:M22)</f>
+        <v>323.69682555555551</v>
       </c>
     </row>
   </sheetData>
@@ -2620,7 +2624,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B8F6C9B-5F1D-4F14-BF34-282173FE9481}">
   <dimension ref="A1:O24"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+    <sheetView zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
       <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
@@ -3194,7 +3198,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91B31920-5678-46E4-B10A-2BE11E7DA4AF}">
   <dimension ref="A1:O23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <selection activeCell="P3" sqref="P3"/>
     </sheetView>
   </sheetViews>
@@ -3403,7 +3407,7 @@
       </c>
       <c r="N11" s="1"/>
       <c r="O11" s="1" t="e">
-        <f t="shared" ref="N11:O11" si="3">AVERAGE(O2:O10)</f>
+        <f t="shared" ref="O11" si="3">AVERAGE(O2:O10)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -3538,7 +3542,7 @@
       </c>
       <c r="B23" s="1"/>
       <c r="C23" s="1" t="e">
-        <f t="shared" ref="B23:C23" si="4">AVERAGE(C14:C22)</f>
+        <f t="shared" ref="C23" si="4">AVERAGE(C14:C22)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="E23" s="1">

</xml_diff>